<commit_message>
human description for the computer-generated masks look like, compared to the human-generated ground truth.
</commit_message>
<xml_diff>
--- a/Segmentation performance.xlsx
+++ b/Segmentation performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Documents\Github\bmen689_group2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E3CC34A-3117-4339-B2F4-A455404BF6B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D06A5B5-93A8-4F63-BC89-DE01C47E954E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4050" yWindow="-11880" windowWidth="14400" windowHeight="7365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="226">
   <si>
     <t>LUNGx-CT001</t>
   </si>
@@ -652,6 +652,57 @@
   </si>
   <si>
     <t>is this correct?</t>
+  </si>
+  <si>
+    <t>decent</t>
+  </si>
+  <si>
+    <t>boundary is bad - detecting lung edge</t>
+  </si>
+  <si>
+    <t>ideas: if elongation is close to 1, delete object</t>
+  </si>
+  <si>
+    <t>TERRIBLE - juxtapleural</t>
+  </si>
+  <si>
+    <t>terrible - juxtapleural</t>
+  </si>
+  <si>
+    <t>use in PPT - almost juxtapleural</t>
+  </si>
+  <si>
+    <t>decent - detecting vessels</t>
+  </si>
+  <si>
+    <t>bad - detecting vessels and lung edge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">decent  </t>
+  </si>
+  <si>
+    <t>decent  small vessel detected</t>
+  </si>
+  <si>
+    <t>decent - lung edge detected despite being juxtapleural</t>
+  </si>
+  <si>
+    <t>floodfill and interior messed up</t>
+  </si>
+  <si>
+    <t>decent - boundary detects lung edges</t>
+  </si>
+  <si>
+    <t>decent - detecting some vessels</t>
+  </si>
+  <si>
+    <t>fix the floodfill mask</t>
+  </si>
+  <si>
+    <t>decent - detecting lung edge</t>
+  </si>
+  <si>
+    <t>TERRIBLE - confused with vessels</t>
   </si>
 </sst>
 </file>
@@ -993,17 +1044,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L72"/>
+  <dimension ref="A1:Q72"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="T57" sqref="T57"/>
+      <selection activeCell="P63" sqref="P63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="0" hidden="1" customWidth="1"/>
-    <col min="3" max="5" width="8.7265625" hidden="1" customWidth="1"/>
-    <col min="6" max="9" width="0" hidden="1" customWidth="1"/>
+    <col min="2" max="9" width="8.7265625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
@@ -1757,7 +1806,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>33</v>
       </c>
@@ -1780,7 +1829,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>34</v>
       </c>
@@ -1803,7 +1852,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>35</v>
       </c>
@@ -1826,7 +1875,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:17" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>36</v>
       </c>
@@ -1849,7 +1898,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:17" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>37</v>
       </c>
@@ -1872,7 +1921,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>38</v>
       </c>
@@ -1895,7 +1944,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>39</v>
       </c>
@@ -1918,7 +1967,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>40</v>
       </c>
@@ -1943,8 +1992,11 @@
       <c r="I40" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="J40" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>41</v>
       </c>
@@ -1966,8 +2018,14 @@
       <c r="I41" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="K41" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>42</v>
       </c>
@@ -1989,8 +2047,11 @@
       <c r="I42" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="K42" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>43</v>
       </c>
@@ -2012,8 +2073,11 @@
       <c r="I43" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="K43" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>44</v>
       </c>
@@ -2035,8 +2099,11 @@
       <c r="I44" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="K44" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>45</v>
       </c>
@@ -2058,8 +2125,14 @@
       <c r="I45" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="K45" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="M45" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>46</v>
       </c>
@@ -2081,8 +2154,14 @@
       <c r="I46" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="K46" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="M46" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>47</v>
       </c>
@@ -2104,8 +2183,11 @@
       <c r="I47" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="K47" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>48</v>
       </c>
@@ -2127,8 +2209,11 @@
       <c r="I48" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="J48" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>49</v>
       </c>
@@ -2150,8 +2235,11 @@
       <c r="I49" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="J49" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>50</v>
       </c>
@@ -2173,8 +2261,11 @@
       <c r="I50" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="K50" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>51</v>
       </c>
@@ -2196,8 +2287,11 @@
       <c r="I51" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="K51" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>52</v>
       </c>
@@ -2219,8 +2313,11 @@
       <c r="I52" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="J52" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>53</v>
       </c>
@@ -2242,8 +2339,11 @@
       <c r="I53" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="J53" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>54</v>
       </c>
@@ -2265,8 +2365,11 @@
       <c r="I54" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="J54" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>55</v>
       </c>
@@ -2288,8 +2391,11 @@
       <c r="I55" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="J55" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>56</v>
       </c>
@@ -2311,8 +2417,14 @@
       <c r="I56" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="J56" t="s">
+        <v>219</v>
+      </c>
+      <c r="K56" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>57</v>
       </c>
@@ -2334,8 +2446,11 @@
       <c r="I57" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="J57" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>58</v>
       </c>
@@ -2360,8 +2475,11 @@
       <c r="I58" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="J58" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>59</v>
       </c>
@@ -2383,8 +2501,11 @@
       <c r="I59" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="J59" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>60</v>
       </c>
@@ -2409,8 +2530,11 @@
       <c r="I60" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="K60" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>61</v>
       </c>
@@ -2432,8 +2556,11 @@
       <c r="I61" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="J61" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>62</v>
       </c>
@@ -2458,8 +2585,11 @@
       <c r="I62" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="J62" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>63</v>
       </c>
@@ -2481,8 +2611,11 @@
       <c r="I63" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="J63" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>64</v>
       </c>
@@ -2504,8 +2637,11 @@
       <c r="I64" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="J64" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>65</v>
       </c>
@@ -2527,8 +2663,11 @@
       <c r="I65" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="K65" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>66</v>
       </c>
@@ -2550,8 +2689,11 @@
       <c r="I66" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="J66" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>67</v>
       </c>
@@ -2573,8 +2715,11 @@
       <c r="I67" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="J67" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>68</v>
       </c>
@@ -2596,8 +2741,14 @@
       <c r="I68" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="K68" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="M68" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>69</v>
       </c>
@@ -2619,8 +2770,11 @@
       <c r="I69" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="J69" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>70</v>
       </c>
@@ -2642,8 +2796,11 @@
       <c r="I70" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="K70" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>71</v>
       </c>
@@ -2665,8 +2822,11 @@
       <c r="I71" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="K71" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A72" s="1"/>
       <c r="B72" t="s">
         <v>205</v>

</xml_diff>